<commit_message>
fixed some mistakes in entries
</commit_message>
<xml_diff>
--- a/Euro2024.xlsx
+++ b/Euro2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\153002\github\pronoseuros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDD4BC4-F253-4986-BECE-5FE0775F5E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE37AE06-C475-41FE-8E35-F320E2C8036D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="943" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="943" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README (2)" sheetId="26" r:id="rId1"/>
@@ -1579,10 +1579,10 @@
     <xf numFmtId="0" fontId="22" fillId="9" borderId="20" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="20" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="20" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="19" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1655,7 +1655,53 @@
     <cellStyle name="Normal 4" xfId="4" xr:uid="{C77B879A-6A24-4C1D-9F97-963E4189EEFE}"/>
     <cellStyle name="Normal 5" xfId="7" xr:uid="{236071A2-3ADA-4BDF-B195-A86731C08A8E}"/>
   </cellStyles>
-  <dxfs count="650">
+  <dxfs count="654">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1673,7 +1719,27 @@
       <font>
         <b val="0"/>
         <i/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
         <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
       </font>
     </dxf>
     <dxf>
@@ -1693,7 +1759,13 @@
       <font>
         <b val="0"/>
         <i/>
-        <color rgb="FF0000FF"/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
       </font>
     </dxf>
     <dxf>
@@ -1705,6 +1777,13 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <color rgb="FF0000FF"/>
@@ -1713,6 +1792,86 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF0000FF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color rgb="FF0000FF"/>
         <family val="2"/>
       </font>
@@ -5541,139 +5700,6 @@
       <font>
         <b/>
         <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF0000FF"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="1" tint="0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="1" tint="0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
@@ -6883,26 +6909,26 @@
     <mergeCell ref="A24:H24"/>
   </mergeCells>
   <conditionalFormatting sqref="E25:E26">
-    <cfRule type="expression" dxfId="649" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="653" priority="1" stopIfTrue="1">
       <formula>#REF!&lt;$G25</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="648" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="652" priority="2" stopIfTrue="1">
       <formula>#REF!&gt;$G25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25:G26">
-    <cfRule type="expression" dxfId="647" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="651" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;$G25</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="646" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="650" priority="4" stopIfTrue="1">
       <formula>#REF!&gt;$G25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25:H26">
-    <cfRule type="expression" dxfId="645" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="649" priority="5" stopIfTrue="1">
       <formula>#REF!&gt;$G25</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="644" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="648" priority="6" stopIfTrue="1">
       <formula>#REF!&lt;$G25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9223,16 +9249,16 @@
       <c r="O51" s="29"/>
     </row>
     <row r="52" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="106"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="29" t="s">
         <v>14</v>
       </c>
@@ -9870,144 +9896,144 @@
     <mergeCell ref="A61:N61"/>
   </mergeCells>
   <conditionalFormatting sqref="E43:E50">
-    <cfRule type="expression" dxfId="357" priority="32">
+    <cfRule type="expression" dxfId="381" priority="32">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="356" priority="31">
+    <cfRule type="expression" dxfId="380" priority="31">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="355" priority="30">
+    <cfRule type="expression" dxfId="379" priority="30">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="354" priority="29">
+    <cfRule type="expression" dxfId="378" priority="29">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E56">
-    <cfRule type="expression" dxfId="353" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="377" priority="1" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="352" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="376" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="351" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="375" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="350" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="374" priority="4" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E60">
-    <cfRule type="expression" dxfId="349" priority="24">
+    <cfRule type="expression" dxfId="373" priority="24">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="348" priority="21">
+    <cfRule type="expression" dxfId="372" priority="21">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="347" priority="22">
+    <cfRule type="expression" dxfId="371" priority="22">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="346" priority="23">
+    <cfRule type="expression" dxfId="370" priority="23">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="345" priority="13">
+    <cfRule type="expression" dxfId="369" priority="13">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="344" priority="14">
+    <cfRule type="expression" dxfId="368" priority="14">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="343" priority="15">
+    <cfRule type="expression" dxfId="367" priority="15">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="342" priority="16">
+    <cfRule type="expression" dxfId="366" priority="16">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:G21 E23:G27">
-    <cfRule type="expression" dxfId="339" priority="37">
+    <cfRule type="expression" dxfId="363" priority="37">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="338" priority="38">
+    <cfRule type="expression" dxfId="362" priority="38">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H21 H23:H27">
-    <cfRule type="expression" dxfId="335" priority="39">
+    <cfRule type="expression" dxfId="359" priority="39">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="334" priority="40">
+    <cfRule type="expression" dxfId="358" priority="40">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50">
-    <cfRule type="expression" dxfId="333" priority="33">
+    <cfRule type="expression" dxfId="357" priority="33">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="332" priority="35">
+    <cfRule type="expression" dxfId="356" priority="35">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="331" priority="36">
+    <cfRule type="expression" dxfId="355" priority="36">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="330" priority="34">
+    <cfRule type="expression" dxfId="354" priority="34">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:H54 H56">
-    <cfRule type="expression" dxfId="329" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="353" priority="7" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="328" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="352" priority="8" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="327" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="351" priority="6" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="326" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="350" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="325" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="349" priority="10" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="324" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="348" priority="9" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="323" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="347" priority="12" stopIfTrue="1">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="322" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="346" priority="11" stopIfTrue="1">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H60">
-    <cfRule type="expression" dxfId="321" priority="25">
+    <cfRule type="expression" dxfId="345" priority="25">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="320" priority="26">
+    <cfRule type="expression" dxfId="344" priority="26">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="319" priority="27">
+    <cfRule type="expression" dxfId="343" priority="27">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="318" priority="28">
+    <cfRule type="expression" dxfId="342" priority="28">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="317" priority="20">
+    <cfRule type="expression" dxfId="341" priority="20">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="316" priority="18">
+    <cfRule type="expression" dxfId="340" priority="18">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="315" priority="19">
+    <cfRule type="expression" dxfId="339" priority="19">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="314" priority="17">
+    <cfRule type="expression" dxfId="338" priority="17">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10071,8 +10097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D45B07A-769B-46B1-A073-DAF4CB3729D0}">
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:H61"/>
+    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -12477,16 +12503,16 @@
       <c r="O51" s="29"/>
     </row>
     <row r="52" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="106"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="29" t="s">
         <v>14</v>
       </c>
@@ -13124,144 +13150,144 @@
     <mergeCell ref="A61:N61"/>
   </mergeCells>
   <conditionalFormatting sqref="E43:E50">
-    <cfRule type="expression" dxfId="313" priority="32">
+    <cfRule type="expression" dxfId="337" priority="32">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="312" priority="31">
+    <cfRule type="expression" dxfId="336" priority="31">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="311" priority="30">
+    <cfRule type="expression" dxfId="335" priority="30">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="310" priority="29">
+    <cfRule type="expression" dxfId="334" priority="29">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E56">
-    <cfRule type="expression" dxfId="309" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="333" priority="1" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="308" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="332" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="307" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="331" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="306" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="330" priority="4" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E60">
-    <cfRule type="expression" dxfId="305" priority="24">
+    <cfRule type="expression" dxfId="329" priority="24">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="304" priority="21">
+    <cfRule type="expression" dxfId="328" priority="21">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="303" priority="22">
+    <cfRule type="expression" dxfId="327" priority="22">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="302" priority="23">
+    <cfRule type="expression" dxfId="326" priority="23">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="301" priority="13">
+    <cfRule type="expression" dxfId="325" priority="13">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="300" priority="14">
+    <cfRule type="expression" dxfId="324" priority="14">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="299" priority="15">
+    <cfRule type="expression" dxfId="323" priority="15">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="298" priority="16">
+    <cfRule type="expression" dxfId="322" priority="16">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:G21 E23:G27">
-    <cfRule type="expression" dxfId="295" priority="37">
+    <cfRule type="expression" dxfId="319" priority="37">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="294" priority="38">
+    <cfRule type="expression" dxfId="318" priority="38">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H21 H23:H27">
-    <cfRule type="expression" dxfId="291" priority="39">
+    <cfRule type="expression" dxfId="315" priority="39">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="290" priority="40">
+    <cfRule type="expression" dxfId="314" priority="40">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50">
-    <cfRule type="expression" dxfId="289" priority="33">
+    <cfRule type="expression" dxfId="313" priority="33">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="288" priority="35">
+    <cfRule type="expression" dxfId="312" priority="35">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="287" priority="36">
+    <cfRule type="expression" dxfId="311" priority="36">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="286" priority="34">
+    <cfRule type="expression" dxfId="310" priority="34">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:H54 H56">
-    <cfRule type="expression" dxfId="285" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="309" priority="7" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="284" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="308" priority="8" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="283" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="307" priority="6" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="282" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="306" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="281" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="305" priority="10" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="280" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="304" priority="9" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="279" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="303" priority="12" stopIfTrue="1">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="278" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="302" priority="11" stopIfTrue="1">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H60">
-    <cfRule type="expression" dxfId="277" priority="25">
+    <cfRule type="expression" dxfId="301" priority="25">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="276" priority="26">
+    <cfRule type="expression" dxfId="300" priority="26">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="275" priority="27">
+    <cfRule type="expression" dxfId="299" priority="27">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="274" priority="28">
+    <cfRule type="expression" dxfId="298" priority="28">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="273" priority="20">
+    <cfRule type="expression" dxfId="297" priority="20">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="272" priority="18">
+    <cfRule type="expression" dxfId="296" priority="18">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="271" priority="19">
+    <cfRule type="expression" dxfId="295" priority="19">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="270" priority="17">
+    <cfRule type="expression" dxfId="294" priority="17">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13325,8 +13351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4B05C9-23F7-47B2-87C5-AA46F1B9CB67}">
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:H61"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -14629,33 +14655,29 @@
       <c r="D29" s="11">
         <v>44367.75</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="9">
-        <v>1</v>
-      </c>
-      <c r="G29" s="9">
-        <v>0</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>28</v>
+      <c r="F29" s="89"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="89" t="s">
+        <v>22</v>
       </c>
       <c r="I29" s="32">
         <f t="shared" ref="I29:I40" si="4">IF(F29&gt;G29,1,IF(F29=G29,2,3))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J29" s="32">
         <f>IF(I29=MAIN!I29,3,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K29" s="33">
         <f t="shared" ref="K29:K40" si="5">F29-G29</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29" s="34">
         <f>IF(K29=MAIN!J29,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29" s="34">
         <f>IF(AND(OJDP!F29=MAIN!F29,OJDP!G29=MAIN!G29),1,0)</f>
@@ -14663,7 +14685,7 @@
       </c>
       <c r="N29" s="31">
         <f>IF(ISBLANK(MAIN!F29),0,J29+L29+M29)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O29" s="29"/>
     </row>
@@ -14680,17 +14702,13 @@
       <c r="D30" s="11">
         <v>44367.75</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" s="9">
-        <v>0</v>
-      </c>
-      <c r="G30" s="9">
-        <v>0</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>29</v>
+      <c r="E30" s="89" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="89" t="s">
+        <v>48</v>
       </c>
       <c r="I30" s="32">
         <f t="shared" si="4"/>
@@ -14731,33 +14749,29 @@
       <c r="D31" s="11">
         <v>44368.75</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F31" s="9">
-        <v>0</v>
-      </c>
-      <c r="G31" s="9">
-        <v>2</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>26</v>
+      <c r="E31" s="89" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="89"/>
+      <c r="G31" s="89"/>
+      <c r="H31" s="89" t="s">
+        <v>25</v>
       </c>
       <c r="I31" s="32">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J31" s="32">
         <f>IF(I31=MAIN!I31,3,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K31" s="33">
         <f t="shared" si="5"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="L31" s="34">
         <f>IF(K31=MAIN!J31,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="34">
         <f>IF(AND(OJDP!F31=MAIN!F31,OJDP!G31=MAIN!G31),1,0)</f>
@@ -14765,7 +14779,7 @@
       </c>
       <c r="N31" s="31">
         <f>IF(ISBLANK(MAIN!F31),0,J31+L31+M31)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O31" s="29"/>
     </row>
@@ -14782,21 +14796,17 @@
       <c r="D32" s="11">
         <v>44368.75</v>
       </c>
-      <c r="E32" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F32" s="9">
-        <v>2</v>
-      </c>
-      <c r="G32" s="9">
-        <v>1</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>39</v>
+      <c r="E32" s="89" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" s="89"/>
+      <c r="G32" s="89"/>
+      <c r="H32" s="89" t="s">
+        <v>24</v>
       </c>
       <c r="I32" s="32">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J32" s="32">
         <f>IF(I32=MAIN!I32,3,0)</f>
@@ -14804,7 +14814,7 @@
       </c>
       <c r="K32" s="33">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L32" s="34">
         <f>IF(K32=MAIN!J32,1,0)</f>
@@ -14833,33 +14843,29 @@
       <c r="D33" s="11">
         <v>44368.875</v>
       </c>
-      <c r="E33" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F33" s="9">
-        <v>0</v>
-      </c>
-      <c r="G33" s="9">
-        <v>1</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>32</v>
+      <c r="E33" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="89"/>
+      <c r="G33" s="89"/>
+      <c r="H33" s="89" t="s">
+        <v>39</v>
       </c>
       <c r="I33" s="32">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J33" s="32">
         <f>IF(I33=MAIN!I33,3,0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K33" s="33">
         <f t="shared" si="5"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L33" s="34">
         <f>IF(K33=MAIN!J33,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33" s="34">
         <f>IF(AND(OJDP!F33=MAIN!F33,OJDP!G33=MAIN!G33),1,0)</f>
@@ -14867,7 +14873,7 @@
       </c>
       <c r="N33" s="31">
         <f>IF(ISBLANK(MAIN!F33),0,J33+L33+M33)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="O33" s="29"/>
     </row>
@@ -14884,17 +14890,13 @@
       <c r="D34" s="11">
         <v>44368.875</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F34" s="9">
-        <v>1</v>
-      </c>
-      <c r="G34" s="9">
-        <v>1</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>34</v>
+      <c r="E34" s="93" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="93"/>
+      <c r="G34" s="93"/>
+      <c r="H34" s="93" t="s">
+        <v>45</v>
       </c>
       <c r="I34" s="32">
         <f t="shared" si="4"/>
@@ -14914,11 +14916,11 @@
       </c>
       <c r="M34" s="34">
         <f>IF(AND(OJDP!F34=MAIN!F34,OJDP!G34=MAIN!G34),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N34" s="31">
         <f>IF(ISBLANK(MAIN!F34),0,J34+L34+M34)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O34" s="29"/>
     </row>
@@ -14935,41 +14937,37 @@
       <c r="D35" s="11">
         <v>44369.875</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F35" s="9">
-        <v>2</v>
-      </c>
-      <c r="G35" s="9">
-        <v>1</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>42</v>
+      <c r="E35" s="89" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="89"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="89" t="s">
+        <v>94</v>
       </c>
       <c r="I35" s="32">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J35" s="32">
         <f>IF(I35=MAIN!I35,3,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K35" s="33">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L35" s="34">
         <f>IF(K35=MAIN!J35,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M35" s="34">
         <f>IF(AND(OJDP!F35=MAIN!F35,OJDP!G35=MAIN!G35),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N35" s="31">
         <f>IF(ISBLANK(MAIN!F35),0,J35+L35+M35)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O35" s="29"/>
     </row>
@@ -14986,41 +14984,37 @@
       <c r="D36" s="11">
         <v>44369.875</v>
       </c>
-      <c r="E36" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F36" s="9">
-        <v>0</v>
-      </c>
-      <c r="G36" s="9">
-        <v>1</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>23</v>
+      <c r="E36" s="89" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="89"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="89" t="s">
+        <v>95</v>
       </c>
       <c r="I36" s="32">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J36" s="32">
         <f>IF(I36=MAIN!I36,3,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K36" s="33">
         <f t="shared" si="5"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L36" s="34">
         <f>IF(K36=MAIN!J36,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M36" s="34">
         <f>IF(AND(OJDP!F36=MAIN!F36,OJDP!G36=MAIN!G36),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N36" s="31">
         <f>IF(ISBLANK(MAIN!F36),0,J36+L36+M36)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O36" s="29"/>
     </row>
@@ -15037,17 +15031,13 @@
       <c r="D37" s="11">
         <v>44370.75</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F37" s="9">
-        <v>1</v>
-      </c>
-      <c r="G37" s="9">
-        <v>1</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>45</v>
+      <c r="E37" s="89" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" s="89"/>
+      <c r="G37" s="89"/>
+      <c r="H37" s="89" t="s">
+        <v>96</v>
       </c>
       <c r="I37" s="32">
         <f t="shared" si="4"/>
@@ -15067,11 +15057,11 @@
       </c>
       <c r="M37" s="34">
         <f>IF(AND(OJDP!F37=MAIN!F37,OJDP!G37=MAIN!G37),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N37" s="31">
         <f>IF(ISBLANK(MAIN!F37),0,J37+L37+M37)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O37" s="29"/>
     </row>
@@ -15088,41 +15078,37 @@
       <c r="D38" s="11">
         <v>44370.75</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F38" s="9">
-        <v>0</v>
-      </c>
-      <c r="G38" s="9">
-        <v>2</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>24</v>
+      <c r="E38" s="89" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" s="89"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="89" t="s">
+        <v>34</v>
       </c>
       <c r="I38" s="32">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J38" s="32">
         <f>IF(I38=MAIN!I38,3,0)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K38" s="33">
         <f t="shared" si="5"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="L38" s="34">
         <f>IF(K38=MAIN!J38,1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" s="34">
         <f>IF(AND(OJDP!F38=MAIN!F38,OJDP!G38=MAIN!G38),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N38" s="31">
         <f>IF(ISBLANK(MAIN!F38),0,J38+L38+M38)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O38" s="29"/>
     </row>
@@ -15139,41 +15125,37 @@
       <c r="D39" s="11">
         <v>44370.875</v>
       </c>
-      <c r="E39" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="F39" s="12">
-        <v>1</v>
-      </c>
-      <c r="G39" s="12">
-        <v>2</v>
-      </c>
-      <c r="H39" s="12" t="s">
-        <v>20</v>
+      <c r="E39" s="89" t="s">
+        <v>97</v>
+      </c>
+      <c r="F39" s="89"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="89" t="s">
+        <v>28</v>
       </c>
       <c r="I39" s="32">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J39" s="32">
         <f>IF(I39=MAIN!I39,3,0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K39" s="33">
         <f t="shared" si="5"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="L39" s="34">
         <f>IF(K39=MAIN!J39,1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39" s="34">
         <f>IF(AND(OJDP!F39=MAIN!F39,OJDP!G39=MAIN!G39),1,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N39" s="31">
         <f>IF(ISBLANK(MAIN!F39),0,J39+L39+M39)*2</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O39" s="29"/>
     </row>
@@ -15190,29 +15172,25 @@
       <c r="D40" s="11">
         <v>44370.875</v>
       </c>
-      <c r="E40" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F40" s="9">
-        <v>3</v>
-      </c>
-      <c r="G40" s="9">
-        <v>0</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>48</v>
+      <c r="E40" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="F40" s="89"/>
+      <c r="G40" s="89"/>
+      <c r="H40" s="89" t="s">
+        <v>82</v>
       </c>
       <c r="I40" s="32">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J40" s="32">
         <f>IF(I40=MAIN!I40,3,0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K40" s="33">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L40" s="34">
         <f>IF(K40=MAIN!J40,1,0)</f>
@@ -15224,11 +15202,11 @@
       </c>
       <c r="N40" s="31">
         <f>IF(ISBLANK(MAIN!F40),0,J40+L40+M40)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O40" s="35">
         <f>SUM(N29:N40)</f>
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -15666,16 +15644,16 @@
       <c r="O51" s="29"/>
     </row>
     <row r="52" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="106"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="29" t="s">
         <v>14</v>
       </c>
@@ -16313,144 +16291,144 @@
     <mergeCell ref="A61:N61"/>
   </mergeCells>
   <conditionalFormatting sqref="E43:E50">
-    <cfRule type="expression" dxfId="269" priority="32">
+    <cfRule type="expression" dxfId="293" priority="36">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="268" priority="31">
+    <cfRule type="expression" dxfId="292" priority="35">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="267" priority="30">
+    <cfRule type="expression" dxfId="291" priority="34">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="266" priority="29">
+    <cfRule type="expression" dxfId="290" priority="33">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E56">
-    <cfRule type="expression" dxfId="265" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="289" priority="5" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="264" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="288" priority="6" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="263" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="287" priority="7" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="262" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="286" priority="8" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E60">
-    <cfRule type="expression" dxfId="261" priority="24">
+    <cfRule type="expression" dxfId="285" priority="28">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="260" priority="21">
+    <cfRule type="expression" dxfId="284" priority="25">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="259" priority="22">
+    <cfRule type="expression" dxfId="283" priority="26">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="258" priority="23">
+    <cfRule type="expression" dxfId="282" priority="27">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="257" priority="13">
+    <cfRule type="expression" dxfId="281" priority="17">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="256" priority="14">
+    <cfRule type="expression" dxfId="280" priority="18">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="255" priority="15">
+    <cfRule type="expression" dxfId="279" priority="19">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="254" priority="16">
+    <cfRule type="expression" dxfId="278" priority="20">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:G21 E23:G27">
-    <cfRule type="expression" dxfId="251" priority="37">
+    <cfRule type="expression" dxfId="275" priority="41">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="250" priority="38">
+    <cfRule type="expression" dxfId="274" priority="42">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H21 H23:H27">
-    <cfRule type="expression" dxfId="247" priority="39">
+    <cfRule type="expression" dxfId="271" priority="43">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="246" priority="40">
+    <cfRule type="expression" dxfId="270" priority="44">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50">
-    <cfRule type="expression" dxfId="245" priority="33">
+    <cfRule type="expression" dxfId="269" priority="37">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="244" priority="35">
+    <cfRule type="expression" dxfId="268" priority="39">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="243" priority="36">
+    <cfRule type="expression" dxfId="267" priority="40">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="242" priority="34">
+    <cfRule type="expression" dxfId="266" priority="38">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:H54 H56">
-    <cfRule type="expression" dxfId="241" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="265" priority="11" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="240" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="264" priority="12" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="239" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="263" priority="10" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="238" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="262" priority="9" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="237" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="261" priority="14" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="236" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="260" priority="13" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="235" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="259" priority="16" stopIfTrue="1">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="234" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="258" priority="15" stopIfTrue="1">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H60">
-    <cfRule type="expression" dxfId="233" priority="25">
+    <cfRule type="expression" dxfId="257" priority="29">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="232" priority="26">
+    <cfRule type="expression" dxfId="256" priority="30">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="231" priority="27">
+    <cfRule type="expression" dxfId="255" priority="31">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="230" priority="28">
+    <cfRule type="expression" dxfId="254" priority="32">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="229" priority="20">
+    <cfRule type="expression" dxfId="253" priority="24">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="228" priority="18">
+    <cfRule type="expression" dxfId="252" priority="22">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="227" priority="19">
+    <cfRule type="expression" dxfId="251" priority="23">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="226" priority="17">
+    <cfRule type="expression" dxfId="250" priority="21">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16461,7 +16439,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="57" id="{8B33D01D-F9FB-4EAA-A45E-481686B5B3D9}">
+          <x14:cfRule type="expression" priority="61" id="{8B33D01D-F9FB-4EAA-A45E-481686B5B3D9}">
             <xm:f>MAIN!#REF!&lt;MAIN!$G3</xm:f>
             <x14:dxf>
               <font>
@@ -16471,7 +16449,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="58" id="{B21591BE-6E10-4CF4-99B8-C7C12A54C238}">
+          <x14:cfRule type="expression" priority="62" id="{B21591BE-6E10-4CF4-99B8-C7C12A54C238}">
             <xm:f>MAIN!#REF!&gt;MAIN!$G3</xm:f>
             <x14:dxf>
               <font>
@@ -16480,10 +16458,10 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E3:G14 E29:G40</xm:sqref>
+          <xm:sqref>E3:G14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="60" id="{624A1F1F-3197-4776-A338-76A0D516F4FE}">
+          <x14:cfRule type="expression" priority="64" id="{624A1F1F-3197-4776-A338-76A0D516F4FE}">
             <xm:f>MAIN!#REF!&lt;MAIN!$G3</xm:f>
             <x14:dxf>
               <font>
@@ -16492,7 +16470,7 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="expression" priority="59" id="{D49D1D12-AAB0-4C2D-A830-F537B4A37A3C}">
+          <x14:cfRule type="expression" priority="63" id="{D49D1D12-AAB0-4C2D-A830-F537B4A37A3C}">
             <xm:f>MAIN!#REF!&gt;MAIN!$G3</xm:f>
             <x14:dxf>
               <font>
@@ -16502,7 +16480,51 @@
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>H3:H14 H29:H40</xm:sqref>
+          <xm:sqref>H3:H14</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{03C5EAFF-4D44-4CE3-AEDB-1EAC25FBFC91}">
+            <xm:f>MAIN!#REF!&lt;MAIN!$G29</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i/>
+                <color theme="1" tint="0.499984740745262"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="2" id="{50097E7D-FF34-4DED-BD42-F248BF56BE84}">
+            <xm:f>MAIN!#REF!&gt;MAIN!$G29</xm:f>
+            <x14:dxf>
+              <font>
+                <b/>
+                <i val="0"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>E29:G40</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="3" id="{610DD319-5D86-49D9-AD33-6A16E1995C5F}">
+            <xm:f>MAIN!#REF!&gt;MAIN!$G29</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i/>
+                <color theme="1" tint="0.499984740745262"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="expression" priority="4" id="{E2F352FA-C852-4CCB-913C-9834AD3014DB}">
+            <xm:f>MAIN!#REF!&lt;MAIN!$G29</xm:f>
+            <x14:dxf>
+              <font>
+                <b/>
+                <i val="0"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>H29:H40</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -18920,16 +18942,16 @@
       <c r="O51" s="29"/>
     </row>
     <row r="52" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="106"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="29" t="s">
         <v>14</v>
       </c>
@@ -19567,144 +19589,144 @@
     <mergeCell ref="A61:N61"/>
   </mergeCells>
   <conditionalFormatting sqref="E43:E50">
-    <cfRule type="expression" dxfId="225" priority="32">
+    <cfRule type="expression" dxfId="249" priority="32">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="224" priority="31">
+    <cfRule type="expression" dxfId="248" priority="31">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="223" priority="30">
+    <cfRule type="expression" dxfId="247" priority="30">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="222" priority="29">
+    <cfRule type="expression" dxfId="246" priority="29">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E56">
-    <cfRule type="expression" dxfId="221" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="245" priority="1" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="220" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="244" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="219" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="243" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="218" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="242" priority="4" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E60">
-    <cfRule type="expression" dxfId="217" priority="24">
+    <cfRule type="expression" dxfId="241" priority="24">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="216" priority="21">
+    <cfRule type="expression" dxfId="240" priority="21">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="215" priority="22">
+    <cfRule type="expression" dxfId="239" priority="22">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="214" priority="23">
+    <cfRule type="expression" dxfId="238" priority="23">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="213" priority="13">
+    <cfRule type="expression" dxfId="237" priority="13">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="212" priority="14">
+    <cfRule type="expression" dxfId="236" priority="14">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="211" priority="15">
+    <cfRule type="expression" dxfId="235" priority="15">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="210" priority="16">
+    <cfRule type="expression" dxfId="234" priority="16">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:G21 E23:G27">
-    <cfRule type="expression" dxfId="207" priority="37">
+    <cfRule type="expression" dxfId="231" priority="37">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="206" priority="38">
+    <cfRule type="expression" dxfId="230" priority="38">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H21 H23:H27">
-    <cfRule type="expression" dxfId="203" priority="39">
+    <cfRule type="expression" dxfId="227" priority="39">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="202" priority="40">
+    <cfRule type="expression" dxfId="226" priority="40">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50">
-    <cfRule type="expression" dxfId="201" priority="33">
+    <cfRule type="expression" dxfId="225" priority="33">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="35">
+    <cfRule type="expression" dxfId="224" priority="35">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="199" priority="36">
+    <cfRule type="expression" dxfId="223" priority="36">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="34">
+    <cfRule type="expression" dxfId="222" priority="34">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:H54 H56">
-    <cfRule type="expression" dxfId="197" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="221" priority="7" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="220" priority="8" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="219" priority="6" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="194" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="218" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="193" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="217" priority="10" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="216" priority="9" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="191" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="215" priority="12" stopIfTrue="1">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="190" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="214" priority="11" stopIfTrue="1">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H60">
-    <cfRule type="expression" dxfId="189" priority="25">
+    <cfRule type="expression" dxfId="213" priority="25">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="188" priority="26">
+    <cfRule type="expression" dxfId="212" priority="26">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="27">
+    <cfRule type="expression" dxfId="211" priority="27">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="28">
+    <cfRule type="expression" dxfId="210" priority="28">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="185" priority="20">
+    <cfRule type="expression" dxfId="209" priority="20">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="18">
+    <cfRule type="expression" dxfId="208" priority="18">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="183" priority="19">
+    <cfRule type="expression" dxfId="207" priority="19">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="182" priority="17">
+    <cfRule type="expression" dxfId="206" priority="17">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22165,16 +22187,16 @@
       <c r="O51" s="29"/>
     </row>
     <row r="52" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="106"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="29" t="s">
         <v>14</v>
       </c>
@@ -22812,144 +22834,144 @@
     <mergeCell ref="A61:N61"/>
   </mergeCells>
   <conditionalFormatting sqref="E43:E50">
-    <cfRule type="expression" dxfId="181" priority="32">
+    <cfRule type="expression" dxfId="205" priority="32">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="31">
+    <cfRule type="expression" dxfId="204" priority="31">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="179" priority="30">
+    <cfRule type="expression" dxfId="203" priority="30">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="29">
+    <cfRule type="expression" dxfId="202" priority="29">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E56">
-    <cfRule type="expression" dxfId="177" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="201" priority="1" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="176" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="200" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="175" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="199" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="198" priority="4" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E60">
-    <cfRule type="expression" dxfId="173" priority="24">
+    <cfRule type="expression" dxfId="197" priority="24">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="21">
+    <cfRule type="expression" dxfId="196" priority="21">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="22">
+    <cfRule type="expression" dxfId="195" priority="22">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="23">
+    <cfRule type="expression" dxfId="194" priority="23">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="169" priority="13">
+    <cfRule type="expression" dxfId="193" priority="13">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="14">
+    <cfRule type="expression" dxfId="192" priority="14">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="167" priority="15">
+    <cfRule type="expression" dxfId="191" priority="15">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="16">
+    <cfRule type="expression" dxfId="190" priority="16">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:G21 E23:G27">
-    <cfRule type="expression" dxfId="163" priority="37">
+    <cfRule type="expression" dxfId="187" priority="37">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="38">
+    <cfRule type="expression" dxfId="186" priority="38">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H21 H23:H27">
-    <cfRule type="expression" dxfId="159" priority="39">
+    <cfRule type="expression" dxfId="183" priority="39">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="40">
+    <cfRule type="expression" dxfId="182" priority="40">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50">
-    <cfRule type="expression" dxfId="157" priority="33">
+    <cfRule type="expression" dxfId="181" priority="33">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="35">
+    <cfRule type="expression" dxfId="180" priority="35">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="36">
+    <cfRule type="expression" dxfId="179" priority="36">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="34">
+    <cfRule type="expression" dxfId="178" priority="34">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:H54 H56">
-    <cfRule type="expression" dxfId="153" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="177" priority="7" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="176" priority="8" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="175" priority="6" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="174" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="149" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="173" priority="10" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="172" priority="9" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="171" priority="12" stopIfTrue="1">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="170" priority="11" stopIfTrue="1">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H60">
-    <cfRule type="expression" dxfId="145" priority="25">
+    <cfRule type="expression" dxfId="169" priority="25">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="26">
+    <cfRule type="expression" dxfId="168" priority="26">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="27">
+    <cfRule type="expression" dxfId="167" priority="27">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="28">
+    <cfRule type="expression" dxfId="166" priority="28">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="141" priority="20">
+    <cfRule type="expression" dxfId="165" priority="20">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="18">
+    <cfRule type="expression" dxfId="164" priority="18">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="19">
+    <cfRule type="expression" dxfId="163" priority="19">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="17">
+    <cfRule type="expression" dxfId="162" priority="17">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25399,16 +25421,16 @@
       <c r="O51" s="29"/>
     </row>
     <row r="52" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="106"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="29" t="s">
         <v>14</v>
       </c>
@@ -26046,144 +26068,144 @@
     <mergeCell ref="A61:N61"/>
   </mergeCells>
   <conditionalFormatting sqref="E43:E50">
-    <cfRule type="expression" dxfId="137" priority="32">
+    <cfRule type="expression" dxfId="161" priority="32">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="31">
+    <cfRule type="expression" dxfId="160" priority="31">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="30">
+    <cfRule type="expression" dxfId="159" priority="30">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="29">
+    <cfRule type="expression" dxfId="158" priority="29">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E56">
-    <cfRule type="expression" dxfId="133" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="1" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="4" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E60">
-    <cfRule type="expression" dxfId="129" priority="24">
+    <cfRule type="expression" dxfId="153" priority="24">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="21">
+    <cfRule type="expression" dxfId="152" priority="21">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="22">
+    <cfRule type="expression" dxfId="151" priority="22">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="23">
+    <cfRule type="expression" dxfId="150" priority="23">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="125" priority="13">
+    <cfRule type="expression" dxfId="149" priority="13">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="14">
+    <cfRule type="expression" dxfId="148" priority="14">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="15">
+    <cfRule type="expression" dxfId="147" priority="15">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="16">
+    <cfRule type="expression" dxfId="146" priority="16">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:G21 E23:G27">
-    <cfRule type="expression" dxfId="119" priority="37">
+    <cfRule type="expression" dxfId="143" priority="37">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="38">
+    <cfRule type="expression" dxfId="142" priority="38">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H21 H23:H27">
-    <cfRule type="expression" dxfId="115" priority="39">
+    <cfRule type="expression" dxfId="139" priority="39">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="40">
+    <cfRule type="expression" dxfId="138" priority="40">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50">
-    <cfRule type="expression" dxfId="113" priority="33">
+    <cfRule type="expression" dxfId="137" priority="33">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="35">
+    <cfRule type="expression" dxfId="136" priority="35">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="36">
+    <cfRule type="expression" dxfId="135" priority="36">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="34">
+    <cfRule type="expression" dxfId="134" priority="34">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:H54 H56">
-    <cfRule type="expression" dxfId="109" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="7" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="8" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="6" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="105" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="10" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="9" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="12" stopIfTrue="1">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="11" stopIfTrue="1">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H60">
-    <cfRule type="expression" dxfId="101" priority="25">
+    <cfRule type="expression" dxfId="125" priority="25">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="26">
+    <cfRule type="expression" dxfId="124" priority="26">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="27">
+    <cfRule type="expression" dxfId="123" priority="27">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="28">
+    <cfRule type="expression" dxfId="122" priority="28">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="97" priority="20">
+    <cfRule type="expression" dxfId="121" priority="20">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="18">
+    <cfRule type="expression" dxfId="120" priority="18">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="19">
+    <cfRule type="expression" dxfId="119" priority="19">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="17">
+    <cfRule type="expression" dxfId="118" priority="17">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28653,16 +28675,16 @@
       <c r="O51" s="29"/>
     </row>
     <row r="52" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="106"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="29" t="s">
         <v>14</v>
       </c>
@@ -29300,144 +29322,144 @@
     <mergeCell ref="A61:N61"/>
   </mergeCells>
   <conditionalFormatting sqref="E43:E50">
-    <cfRule type="expression" dxfId="93" priority="32">
+    <cfRule type="expression" dxfId="117" priority="32">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="31">
+    <cfRule type="expression" dxfId="116" priority="31">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="30">
+    <cfRule type="expression" dxfId="115" priority="30">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="29">
+    <cfRule type="expression" dxfId="114" priority="29">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E56">
-    <cfRule type="expression" dxfId="89" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="1" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="4" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E60">
-    <cfRule type="expression" dxfId="85" priority="24">
+    <cfRule type="expression" dxfId="109" priority="24">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="21">
+    <cfRule type="expression" dxfId="108" priority="21">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="22">
+    <cfRule type="expression" dxfId="107" priority="22">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="23">
+    <cfRule type="expression" dxfId="106" priority="23">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="81" priority="13">
+    <cfRule type="expression" dxfId="105" priority="13">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="14">
+    <cfRule type="expression" dxfId="104" priority="14">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="15">
+    <cfRule type="expression" dxfId="103" priority="15">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="16">
+    <cfRule type="expression" dxfId="102" priority="16">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:G21 E23:G27">
-    <cfRule type="expression" dxfId="75" priority="37">
+    <cfRule type="expression" dxfId="99" priority="37">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="38">
+    <cfRule type="expression" dxfId="98" priority="38">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H21 H23:H27">
-    <cfRule type="expression" dxfId="71" priority="39">
+    <cfRule type="expression" dxfId="95" priority="39">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="40">
+    <cfRule type="expression" dxfId="94" priority="40">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50">
-    <cfRule type="expression" dxfId="69" priority="33">
+    <cfRule type="expression" dxfId="93" priority="33">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="35">
+    <cfRule type="expression" dxfId="92" priority="35">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="36">
+    <cfRule type="expression" dxfId="91" priority="36">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="34">
+    <cfRule type="expression" dxfId="90" priority="34">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:H54 H56">
-    <cfRule type="expression" dxfId="65" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="7" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="8" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="6" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="61" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="10" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="9" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="12" stopIfTrue="1">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="11" stopIfTrue="1">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H60">
-    <cfRule type="expression" dxfId="57" priority="25">
+    <cfRule type="expression" dxfId="81" priority="25">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="26">
+    <cfRule type="expression" dxfId="80" priority="26">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="27">
+    <cfRule type="expression" dxfId="79" priority="27">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="28">
+    <cfRule type="expression" dxfId="78" priority="28">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="53" priority="20">
+    <cfRule type="expression" dxfId="77" priority="20">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="18">
+    <cfRule type="expression" dxfId="76" priority="18">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="19">
+    <cfRule type="expression" dxfId="75" priority="19">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="17">
+    <cfRule type="expression" dxfId="74" priority="17">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31907,16 +31929,16 @@
       <c r="O51" s="29"/>
     </row>
     <row r="52" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="106"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="29" t="s">
         <v>14</v>
       </c>
@@ -32554,168 +32576,168 @@
     <mergeCell ref="A61:N61"/>
   </mergeCells>
   <conditionalFormatting sqref="E43:E50">
-    <cfRule type="expression" dxfId="47" priority="31">
+    <cfRule type="expression" dxfId="71" priority="31">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="30">
+    <cfRule type="expression" dxfId="70" priority="30">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="32">
+    <cfRule type="expression" dxfId="69" priority="32">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="29">
+    <cfRule type="expression" dxfId="68" priority="29">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E56">
-    <cfRule type="expression" dxfId="43" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="1" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="4" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E60">
-    <cfRule type="expression" dxfId="39" priority="21">
+    <cfRule type="expression" dxfId="63" priority="21">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="22">
+    <cfRule type="expression" dxfId="62" priority="22">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="23">
+    <cfRule type="expression" dxfId="61" priority="23">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="24">
+    <cfRule type="expression" dxfId="60" priority="24">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="35" priority="13">
+    <cfRule type="expression" dxfId="59" priority="13">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="14">
+    <cfRule type="expression" dxfId="58" priority="14">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="15">
+    <cfRule type="expression" dxfId="57" priority="15">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="16">
+    <cfRule type="expression" dxfId="56" priority="16">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:G21 E23:G27">
-    <cfRule type="expression" dxfId="31" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="40" stopIfTrue="1">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="39" stopIfTrue="1">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:G40">
-    <cfRule type="expression" dxfId="29" priority="44">
+    <cfRule type="expression" dxfId="53" priority="44">
       <formula>#REF!&gt;$G29</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="43">
+    <cfRule type="expression" dxfId="52" priority="43">
       <formula>#REF!&lt;$G29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G14">
-    <cfRule type="expression" dxfId="27" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="50" stopIfTrue="1">
       <formula>#REF!&gt;$G3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="49" stopIfTrue="1">
       <formula>#REF!&lt;$G3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H21 H23:H27">
-    <cfRule type="expression" dxfId="23" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="37" stopIfTrue="1">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="38" stopIfTrue="1">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29:H40">
-    <cfRule type="expression" dxfId="21" priority="45">
+    <cfRule type="expression" dxfId="45" priority="45">
       <formula>#REF!&gt;$G29</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="46">
+    <cfRule type="expression" dxfId="44" priority="46">
       <formula>#REF!&lt;$G29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50">
-    <cfRule type="expression" dxfId="19" priority="33">
+    <cfRule type="expression" dxfId="43" priority="33">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="34">
+    <cfRule type="expression" dxfId="42" priority="34">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="35">
+    <cfRule type="expression" dxfId="41" priority="35">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="36">
+    <cfRule type="expression" dxfId="40" priority="36">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:H54 H56">
-    <cfRule type="expression" dxfId="15" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="7" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="8" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="6" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="12" stopIfTrue="1">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="11" stopIfTrue="1">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="10" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="9" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H60">
-    <cfRule type="expression" dxfId="7" priority="25">
+    <cfRule type="expression" dxfId="31" priority="25">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="27">
+    <cfRule type="expression" dxfId="30" priority="27">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="26">
+    <cfRule type="expression" dxfId="29" priority="26">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="28">
+    <cfRule type="expression" dxfId="28" priority="28">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="3" priority="19">
+    <cfRule type="expression" dxfId="27" priority="19">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="18">
+    <cfRule type="expression" dxfId="26" priority="18">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="20">
+    <cfRule type="expression" dxfId="25" priority="20">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="17">
+    <cfRule type="expression" dxfId="24" priority="17">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32779,7 +32801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F893C4-2BAF-42A0-BFC9-8BC22EDB9CAB}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -34605,76 +34627,76 @@
     <mergeCell ref="A61:J61"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E12 E16:G21 E23:G27 E29:G40">
-    <cfRule type="expression" dxfId="599" priority="7">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>#REF!&lt;$G3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="598" priority="8">
+    <cfRule type="expression" dxfId="22" priority="8">
       <formula>#REF!&gt;$G3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="597" priority="11">
+    <cfRule type="expression" dxfId="21" priority="11">
       <formula>#REF!&lt;$G13</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="596" priority="12">
+    <cfRule type="expression" dxfId="20" priority="12">
       <formula>#REF!&gt;$G13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43:E50 E53:E56 E59:E60 E63">
-    <cfRule type="expression" dxfId="595" priority="13">
+    <cfRule type="expression" dxfId="19" priority="13">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="594" priority="14">
+    <cfRule type="expression" dxfId="18" priority="14">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="593" priority="15">
+    <cfRule type="expression" dxfId="17" priority="15">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="592" priority="16">
+    <cfRule type="expression" dxfId="16" priority="16">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G14">
-    <cfRule type="expression" dxfId="591" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>#REF!&lt;$G3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="590" priority="6">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>#REF!&gt;$G3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H14 H16:H21 H23:H27 H29:H40">
-    <cfRule type="expression" dxfId="589" priority="9">
+    <cfRule type="expression" dxfId="13" priority="9">
       <formula>#REF!&gt;$G3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="588" priority="10">
+    <cfRule type="expression" dxfId="12" priority="10">
       <formula>#REF!&lt;$G3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50 H53:H54 H56 H59:H60 H63">
-    <cfRule type="expression" dxfId="587" priority="17">
+    <cfRule type="expression" dxfId="11" priority="17">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="586" priority="18">
+    <cfRule type="expression" dxfId="10" priority="18">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="585" priority="19">
+    <cfRule type="expression" dxfId="9" priority="19">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="584" priority="20">
+    <cfRule type="expression" dxfId="8" priority="20">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="583" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="582" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="581" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="580" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34811,16 +34833,16 @@
       <c r="J6" s="72"/>
     </row>
     <row r="7" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="106"/>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="106"/>
-      <c r="H7" s="106"/>
+      <c r="B7" s="105"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="105"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="105"/>
+      <c r="H7" s="105"/>
       <c r="I7" s="73" t="s">
         <v>137</v>
       </c>
@@ -35114,16 +35136,16 @@
       <c r="J19" s="77"/>
     </row>
     <row r="20" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="105" t="s">
+      <c r="A20" s="106" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="105"/>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="105"/>
-      <c r="F20" s="105"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="105"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="106"/>
+      <c r="F20" s="106"/>
+      <c r="G20" s="106"/>
+      <c r="H20" s="106"/>
       <c r="I20" s="80" t="s">
         <v>138</v>
       </c>
@@ -35417,16 +35439,16 @@
       <c r="J32" s="77"/>
     </row>
     <row r="33" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="105" t="s">
+      <c r="A33" s="106" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="105"/>
-      <c r="C33" s="105"/>
-      <c r="D33" s="105"/>
-      <c r="E33" s="105"/>
-      <c r="F33" s="105"/>
-      <c r="G33" s="105"/>
-      <c r="H33" s="105"/>
+      <c r="B33" s="106"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="106"/>
+      <c r="F33" s="106"/>
+      <c r="G33" s="106"/>
+      <c r="H33" s="106"/>
       <c r="I33" s="73" t="s">
         <v>137</v>
       </c>
@@ -35735,16 +35757,16 @@
       <c r="J46" s="72"/>
     </row>
     <row r="47" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="106" t="s">
+      <c r="A47" s="105" t="s">
         <v>102</v>
       </c>
-      <c r="B47" s="106"/>
-      <c r="C47" s="106"/>
-      <c r="D47" s="106"/>
-      <c r="E47" s="106"/>
-      <c r="F47" s="106"/>
-      <c r="G47" s="106"/>
-      <c r="H47" s="106"/>
+      <c r="B47" s="105"/>
+      <c r="C47" s="105"/>
+      <c r="D47" s="105"/>
+      <c r="E47" s="105"/>
+      <c r="F47" s="105"/>
+      <c r="G47" s="105"/>
+      <c r="H47" s="105"/>
       <c r="I47" s="80" t="s">
         <v>138</v>
       </c>
@@ -35943,16 +35965,16 @@
       <c r="J56" s="72"/>
     </row>
     <row r="57" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A57" s="106" t="s">
+      <c r="A57" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B57" s="106"/>
-      <c r="C57" s="106"/>
-      <c r="D57" s="106"/>
-      <c r="E57" s="106"/>
-      <c r="F57" s="106"/>
-      <c r="G57" s="106"/>
-      <c r="H57" s="106"/>
+      <c r="B57" s="105"/>
+      <c r="C57" s="105"/>
+      <c r="D57" s="105"/>
+      <c r="E57" s="105"/>
+      <c r="F57" s="105"/>
+      <c r="G57" s="105"/>
+      <c r="H57" s="105"/>
       <c r="I57" s="73" t="s">
         <v>137</v>
       </c>
@@ -36063,16 +36085,16 @@
       <c r="J62" s="72"/>
     </row>
     <row r="63" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="106" t="s">
+      <c r="A63" s="105" t="s">
         <v>104</v>
       </c>
-      <c r="B63" s="106"/>
-      <c r="C63" s="106"/>
-      <c r="D63" s="106"/>
-      <c r="E63" s="106"/>
-      <c r="F63" s="106"/>
-      <c r="G63" s="106"/>
-      <c r="H63" s="106"/>
+      <c r="B63" s="105"/>
+      <c r="C63" s="105"/>
+      <c r="D63" s="105"/>
+      <c r="E63" s="105"/>
+      <c r="F63" s="105"/>
+      <c r="G63" s="105"/>
+      <c r="H63" s="105"/>
       <c r="I63" s="80" t="s">
         <v>138</v>
       </c>
@@ -36139,16 +36161,16 @@
       <c r="J66" s="72"/>
     </row>
     <row r="67" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="106" t="s">
+      <c r="A67" s="105" t="s">
         <v>105</v>
       </c>
-      <c r="B67" s="106"/>
-      <c r="C67" s="106"/>
-      <c r="D67" s="106"/>
-      <c r="E67" s="106"/>
-      <c r="F67" s="106"/>
-      <c r="G67" s="106"/>
-      <c r="H67" s="106"/>
+      <c r="B67" s="105"/>
+      <c r="C67" s="105"/>
+      <c r="D67" s="105"/>
+      <c r="E67" s="105"/>
+      <c r="F67" s="105"/>
+      <c r="G67" s="105"/>
+      <c r="H67" s="105"/>
       <c r="I67" s="80" t="s">
         <v>138</v>
       </c>
@@ -36180,11 +36202,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A57:H57"/>
-    <mergeCell ref="A62:H62"/>
-    <mergeCell ref="A63:H63"/>
-    <mergeCell ref="A66:H66"/>
-    <mergeCell ref="A67:H67"/>
     <mergeCell ref="A33:H33"/>
     <mergeCell ref="A46:H46"/>
     <mergeCell ref="A47:H47"/>
@@ -36195,80 +36212,85 @@
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A57:H57"/>
+    <mergeCell ref="A62:H62"/>
+    <mergeCell ref="A63:H63"/>
+    <mergeCell ref="A66:H66"/>
+    <mergeCell ref="A67:H67"/>
   </mergeCells>
   <conditionalFormatting sqref="E8:E17 E21:G26 E28:G32 E34:G45">
-    <cfRule type="expression" dxfId="643" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="647" priority="1" stopIfTrue="1">
       <formula>#REF!&lt;$G8</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="642" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="646" priority="2" stopIfTrue="1">
       <formula>#REF!&gt;$G8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="641" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="645" priority="7" stopIfTrue="1">
       <formula>#REF!&lt;$G18</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="640" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="644" priority="8" stopIfTrue="1">
       <formula>#REF!&gt;$G18</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:E55 E58:E61 E64:E65 E68">
-    <cfRule type="expression" dxfId="639" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="643" priority="9" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="638" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="642" priority="10" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="637" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="641" priority="11" stopIfTrue="1">
       <formula>#REF!&lt;$G48</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="636" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="640" priority="12" stopIfTrue="1">
       <formula>#REF!&gt;$G48</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:G19">
-    <cfRule type="expression" dxfId="635" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="639" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;$G8</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="634" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="638" priority="6" stopIfTrue="1">
       <formula>#REF!&gt;$G8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H19 H21:H26 H28:H32 H34:H45 H48:H55">
-    <cfRule type="expression" dxfId="633" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="637" priority="3" stopIfTrue="1">
       <formula>#REF!&gt;$G8</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="632" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="636" priority="4" stopIfTrue="1">
       <formula>#REF!&lt;$G8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48:H55 H58:H59 H61 H64:H65 H68">
-    <cfRule type="expression" dxfId="631" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="635" priority="13" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="630" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="634" priority="14" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58:H59 H61 H64:H65 H68">
-    <cfRule type="expression" dxfId="629" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="633" priority="15" stopIfTrue="1">
       <formula>#REF!&gt;$G58</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="628" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="632" priority="16" stopIfTrue="1">
       <formula>#REF!&lt;$G58</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H60">
-    <cfRule type="expression" dxfId="627" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="631" priority="17" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="626" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="630" priority="18" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="625" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="629" priority="19" stopIfTrue="1">
       <formula>#REF!&lt;$G60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="624" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="628" priority="20" stopIfTrue="1">
       <formula>#REF!&gt;$G60</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38218,76 +38240,76 @@
     <mergeCell ref="A57:J57"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E12 E29:G40">
-    <cfRule type="expression" dxfId="623" priority="68">
+    <cfRule type="expression" dxfId="627" priority="68">
       <formula>#REF!&lt;$G3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="622" priority="69">
+    <cfRule type="expression" dxfId="626" priority="69">
       <formula>#REF!&gt;$G3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="621" priority="117">
+    <cfRule type="expression" dxfId="625" priority="117">
       <formula>#REF!&lt;$G13</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="620" priority="118">
+    <cfRule type="expression" dxfId="624" priority="118">
       <formula>#REF!&gt;$G13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43:E50 E53:E56 E59:E60 E63">
-    <cfRule type="expression" dxfId="617" priority="1001">
+    <cfRule type="expression" dxfId="621" priority="1001">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="616" priority="1002">
+    <cfRule type="expression" dxfId="620" priority="1002">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="615" priority="1003">
+    <cfRule type="expression" dxfId="619" priority="1003">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="614" priority="1004">
+    <cfRule type="expression" dxfId="618" priority="1004">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G14">
-    <cfRule type="expression" dxfId="613" priority="5">
+    <cfRule type="expression" dxfId="617" priority="5">
       <formula>#REF!&lt;$G3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="612" priority="6">
+    <cfRule type="expression" dxfId="616" priority="6">
       <formula>#REF!&gt;$G3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H14 H29:H40">
-    <cfRule type="expression" dxfId="611" priority="70">
+    <cfRule type="expression" dxfId="615" priority="70">
       <formula>#REF!&gt;$G3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="610" priority="71">
+    <cfRule type="expression" dxfId="614" priority="71">
       <formula>#REF!&lt;$G3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50 H53:H54 H56 H59:H60 H63">
-    <cfRule type="expression" dxfId="607" priority="1017">
+    <cfRule type="expression" dxfId="611" priority="1017">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="606" priority="1018">
+    <cfRule type="expression" dxfId="610" priority="1018">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="605" priority="1019">
+    <cfRule type="expression" dxfId="609" priority="1019">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="604" priority="1020">
+    <cfRule type="expression" dxfId="608" priority="1020">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="603" priority="1">
+    <cfRule type="expression" dxfId="607" priority="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="602" priority="2">
+    <cfRule type="expression" dxfId="606" priority="2">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="601" priority="3">
+    <cfRule type="expression" dxfId="605" priority="3">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="600" priority="4">
+    <cfRule type="expression" dxfId="604" priority="4">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38781,7 +38803,7 @@
       </c>
       <c r="C11" s="51">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D11" s="5">
         <f>OJDP!$O$14</f>
@@ -38793,7 +38815,7 @@
       </c>
       <c r="F11" s="2">
         <f>OJDP!O40</f>
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G11" s="4" t="e">
         <f>#REF!</f>
@@ -41576,16 +41598,16 @@
       <c r="O51" s="29"/>
     </row>
     <row r="52" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="106"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="29" t="s">
         <v>14</v>
       </c>
@@ -42223,152 +42245,152 @@
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="E43:E50">
-    <cfRule type="expression" dxfId="577" priority="44">
+    <cfRule type="expression" dxfId="601" priority="44">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="576" priority="43">
+    <cfRule type="expression" dxfId="600" priority="43">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="575" priority="41">
+    <cfRule type="expression" dxfId="599" priority="41">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="574" priority="42">
+    <cfRule type="expression" dxfId="598" priority="42">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E56">
-    <cfRule type="expression" dxfId="573" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="597" priority="1" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="572" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="596" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="571" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="595" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="570" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="594" priority="4" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E60">
-    <cfRule type="expression" dxfId="569" priority="23">
+    <cfRule type="expression" dxfId="593" priority="23">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="568" priority="24">
+    <cfRule type="expression" dxfId="592" priority="24">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="567" priority="21">
+    <cfRule type="expression" dxfId="591" priority="21">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="566" priority="22">
+    <cfRule type="expression" dxfId="590" priority="22">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="565" priority="13">
+    <cfRule type="expression" dxfId="589" priority="13">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="564" priority="14">
+    <cfRule type="expression" dxfId="588" priority="14">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="563" priority="15">
+    <cfRule type="expression" dxfId="587" priority="15">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="562" priority="16">
+    <cfRule type="expression" dxfId="586" priority="16">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:G21 E23:G27">
-    <cfRule type="expression" dxfId="561" priority="50">
+    <cfRule type="expression" dxfId="585" priority="50">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="560" priority="49">
+    <cfRule type="expression" dxfId="584" priority="49">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G14">
-    <cfRule type="expression" dxfId="559" priority="62">
+    <cfRule type="expression" dxfId="583" priority="62">
       <formula>#REF!&gt;$G3</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="558" priority="61">
+    <cfRule type="expression" dxfId="582" priority="61">
       <formula>#REF!&lt;$G3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H21 H23:H27">
-    <cfRule type="expression" dxfId="555" priority="51">
+    <cfRule type="expression" dxfId="579" priority="51">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="554" priority="52">
+    <cfRule type="expression" dxfId="578" priority="52">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50">
-    <cfRule type="expression" dxfId="553" priority="45">
+    <cfRule type="expression" dxfId="577" priority="45">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="552" priority="46">
+    <cfRule type="expression" dxfId="576" priority="46">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="551" priority="47">
+    <cfRule type="expression" dxfId="575" priority="47">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="550" priority="48">
+    <cfRule type="expression" dxfId="574" priority="48">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:H54 H56">
-    <cfRule type="expression" dxfId="549" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="573" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="548" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="572" priority="6" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="547" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="571" priority="8" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="546" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="570" priority="7" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="545" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="569" priority="12" stopIfTrue="1">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="544" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="568" priority="11" stopIfTrue="1">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="543" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="567" priority="10" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="542" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="566" priority="9" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H60">
-    <cfRule type="expression" dxfId="541" priority="26">
+    <cfRule type="expression" dxfId="565" priority="26">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="540" priority="27">
+    <cfRule type="expression" dxfId="564" priority="27">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="539" priority="28">
+    <cfRule type="expression" dxfId="563" priority="28">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="538" priority="25">
+    <cfRule type="expression" dxfId="562" priority="25">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="537" priority="19">
+    <cfRule type="expression" dxfId="561" priority="19">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="536" priority="20">
+    <cfRule type="expression" dxfId="560" priority="20">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="535" priority="18">
+    <cfRule type="expression" dxfId="559" priority="18">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="534" priority="17">
+    <cfRule type="expression" dxfId="558" priority="17">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -44838,16 +44860,16 @@
       <c r="O51" s="29"/>
     </row>
     <row r="52" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="106"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="29" t="s">
         <v>14</v>
       </c>
@@ -45485,144 +45507,144 @@
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="E43:E50">
-    <cfRule type="expression" dxfId="533" priority="32">
+    <cfRule type="expression" dxfId="557" priority="32">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="532" priority="31">
+    <cfRule type="expression" dxfId="556" priority="31">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="531" priority="30">
+    <cfRule type="expression" dxfId="555" priority="30">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="530" priority="29">
+    <cfRule type="expression" dxfId="554" priority="29">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E56">
-    <cfRule type="expression" dxfId="529" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="553" priority="1" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="528" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="552" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="527" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="551" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="526" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="550" priority="4" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E60">
-    <cfRule type="expression" dxfId="525" priority="24">
+    <cfRule type="expression" dxfId="549" priority="24">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="524" priority="21">
+    <cfRule type="expression" dxfId="548" priority="21">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="523" priority="22">
+    <cfRule type="expression" dxfId="547" priority="22">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="522" priority="23">
+    <cfRule type="expression" dxfId="546" priority="23">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="521" priority="13">
+    <cfRule type="expression" dxfId="545" priority="13">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="520" priority="14">
+    <cfRule type="expression" dxfId="544" priority="14">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="519" priority="15">
+    <cfRule type="expression" dxfId="543" priority="15">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="518" priority="16">
+    <cfRule type="expression" dxfId="542" priority="16">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:G21 E23:G27">
-    <cfRule type="expression" dxfId="515" priority="37">
+    <cfRule type="expression" dxfId="539" priority="37">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="514" priority="38">
+    <cfRule type="expression" dxfId="538" priority="38">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H21 H23:H27">
-    <cfRule type="expression" dxfId="511" priority="39">
+    <cfRule type="expression" dxfId="535" priority="39">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="510" priority="40">
+    <cfRule type="expression" dxfId="534" priority="40">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50">
-    <cfRule type="expression" dxfId="509" priority="33">
+    <cfRule type="expression" dxfId="533" priority="33">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="508" priority="35">
+    <cfRule type="expression" dxfId="532" priority="35">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="507" priority="36">
+    <cfRule type="expression" dxfId="531" priority="36">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="506" priority="34">
+    <cfRule type="expression" dxfId="530" priority="34">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:H54 H56">
-    <cfRule type="expression" dxfId="505" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="529" priority="7" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="504" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="528" priority="8" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="503" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="527" priority="6" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="502" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="526" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="501" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="525" priority="10" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="500" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="524" priority="9" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="499" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="523" priority="12" stopIfTrue="1">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="498" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="522" priority="11" stopIfTrue="1">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H60">
-    <cfRule type="expression" dxfId="497" priority="25">
+    <cfRule type="expression" dxfId="521" priority="25">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="496" priority="26">
+    <cfRule type="expression" dxfId="520" priority="26">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="495" priority="27">
+    <cfRule type="expression" dxfId="519" priority="27">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="494" priority="28">
+    <cfRule type="expression" dxfId="518" priority="28">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="493" priority="20">
+    <cfRule type="expression" dxfId="517" priority="20">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="492" priority="18">
+    <cfRule type="expression" dxfId="516" priority="18">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="491" priority="19">
+    <cfRule type="expression" dxfId="515" priority="19">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="490" priority="17">
+    <cfRule type="expression" dxfId="514" priority="17">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -48055,16 +48077,16 @@
       <c r="O51" s="29"/>
     </row>
     <row r="52" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="106"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="29" t="s">
         <v>14</v>
       </c>
@@ -48702,144 +48724,144 @@
     <mergeCell ref="A61:N61"/>
   </mergeCells>
   <conditionalFormatting sqref="E43:E50">
-    <cfRule type="expression" dxfId="489" priority="32">
+    <cfRule type="expression" dxfId="513" priority="32">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="488" priority="31">
+    <cfRule type="expression" dxfId="512" priority="31">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="487" priority="30">
+    <cfRule type="expression" dxfId="511" priority="30">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="486" priority="29">
+    <cfRule type="expression" dxfId="510" priority="29">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E56">
-    <cfRule type="expression" dxfId="485" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="509" priority="1" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="484" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="508" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="483" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="507" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="482" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="506" priority="4" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E60">
-    <cfRule type="expression" dxfId="481" priority="24">
+    <cfRule type="expression" dxfId="505" priority="24">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="480" priority="21">
+    <cfRule type="expression" dxfId="504" priority="21">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="479" priority="22">
+    <cfRule type="expression" dxfId="503" priority="22">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="478" priority="23">
+    <cfRule type="expression" dxfId="502" priority="23">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="477" priority="13">
+    <cfRule type="expression" dxfId="501" priority="13">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="476" priority="14">
+    <cfRule type="expression" dxfId="500" priority="14">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="475" priority="15">
+    <cfRule type="expression" dxfId="499" priority="15">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="474" priority="16">
+    <cfRule type="expression" dxfId="498" priority="16">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:G21 E23:G27">
-    <cfRule type="expression" dxfId="471" priority="37">
+    <cfRule type="expression" dxfId="495" priority="37">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="470" priority="38">
+    <cfRule type="expression" dxfId="494" priority="38">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H21 H23:H27">
-    <cfRule type="expression" dxfId="467" priority="39">
+    <cfRule type="expression" dxfId="491" priority="39">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="466" priority="40">
+    <cfRule type="expression" dxfId="490" priority="40">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50">
-    <cfRule type="expression" dxfId="465" priority="33">
+    <cfRule type="expression" dxfId="489" priority="33">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="464" priority="35">
+    <cfRule type="expression" dxfId="488" priority="35">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="463" priority="36">
+    <cfRule type="expression" dxfId="487" priority="36">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="462" priority="34">
+    <cfRule type="expression" dxfId="486" priority="34">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:H54 H56">
-    <cfRule type="expression" dxfId="461" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="485" priority="7" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="460" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="484" priority="8" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="459" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="483" priority="6" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="458" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="482" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="457" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="481" priority="10" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="456" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="480" priority="9" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="455" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="479" priority="12" stopIfTrue="1">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="454" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="478" priority="11" stopIfTrue="1">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H60">
-    <cfRule type="expression" dxfId="453" priority="25">
+    <cfRule type="expression" dxfId="477" priority="25">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="452" priority="26">
+    <cfRule type="expression" dxfId="476" priority="26">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="451" priority="27">
+    <cfRule type="expression" dxfId="475" priority="27">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="450" priority="28">
+    <cfRule type="expression" dxfId="474" priority="28">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="449" priority="20">
+    <cfRule type="expression" dxfId="473" priority="20">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="448" priority="18">
+    <cfRule type="expression" dxfId="472" priority="18">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="447" priority="19">
+    <cfRule type="expression" dxfId="471" priority="19">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="446" priority="17">
+    <cfRule type="expression" dxfId="470" priority="17">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -51309,16 +51331,16 @@
       <c r="O51" s="29"/>
     </row>
     <row r="52" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="106"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="29" t="s">
         <v>14</v>
       </c>
@@ -51956,144 +51978,144 @@
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="E43:E50">
-    <cfRule type="expression" dxfId="445" priority="32">
+    <cfRule type="expression" dxfId="469" priority="32">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="444" priority="31">
+    <cfRule type="expression" dxfId="468" priority="31">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="443" priority="30">
+    <cfRule type="expression" dxfId="467" priority="30">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="442" priority="29">
+    <cfRule type="expression" dxfId="466" priority="29">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E56">
-    <cfRule type="expression" dxfId="441" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="465" priority="1" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="440" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="464" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="439" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="463" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="438" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="462" priority="4" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E60">
-    <cfRule type="expression" dxfId="437" priority="24">
+    <cfRule type="expression" dxfId="461" priority="24">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="436" priority="21">
+    <cfRule type="expression" dxfId="460" priority="21">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="435" priority="22">
+    <cfRule type="expression" dxfId="459" priority="22">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="434" priority="23">
+    <cfRule type="expression" dxfId="458" priority="23">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="433" priority="13">
+    <cfRule type="expression" dxfId="457" priority="13">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="432" priority="14">
+    <cfRule type="expression" dxfId="456" priority="14">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="431" priority="15">
+    <cfRule type="expression" dxfId="455" priority="15">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="430" priority="16">
+    <cfRule type="expression" dxfId="454" priority="16">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:G21 E23:G27">
-    <cfRule type="expression" dxfId="427" priority="37">
+    <cfRule type="expression" dxfId="451" priority="37">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="426" priority="38">
+    <cfRule type="expression" dxfId="450" priority="38">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H21 H23:H27">
-    <cfRule type="expression" dxfId="423" priority="39">
+    <cfRule type="expression" dxfId="447" priority="39">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="422" priority="40">
+    <cfRule type="expression" dxfId="446" priority="40">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50">
-    <cfRule type="expression" dxfId="421" priority="33">
+    <cfRule type="expression" dxfId="445" priority="33">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="420" priority="35">
+    <cfRule type="expression" dxfId="444" priority="35">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="419" priority="36">
+    <cfRule type="expression" dxfId="443" priority="36">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="418" priority="34">
+    <cfRule type="expression" dxfId="442" priority="34">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:H54 H56">
-    <cfRule type="expression" dxfId="417" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="441" priority="7" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="416" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="440" priority="8" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="415" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="439" priority="6" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="414" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="438" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="413" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="437" priority="10" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="412" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="436" priority="9" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="411" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="435" priority="12" stopIfTrue="1">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="410" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="434" priority="11" stopIfTrue="1">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H60">
-    <cfRule type="expression" dxfId="409" priority="25">
+    <cfRule type="expression" dxfId="433" priority="25">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="408" priority="26">
+    <cfRule type="expression" dxfId="432" priority="26">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="407" priority="27">
+    <cfRule type="expression" dxfId="431" priority="27">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="406" priority="28">
+    <cfRule type="expression" dxfId="430" priority="28">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="405" priority="20">
+    <cfRule type="expression" dxfId="429" priority="20">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="404" priority="18">
+    <cfRule type="expression" dxfId="428" priority="18">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="403" priority="19">
+    <cfRule type="expression" dxfId="427" priority="19">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="402" priority="17">
+    <cfRule type="expression" dxfId="426" priority="17">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -54563,16 +54585,16 @@
       <c r="O51" s="29"/>
     </row>
     <row r="52" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="106" t="s">
+      <c r="A52" s="105" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="106"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
       <c r="I52" s="29" t="s">
         <v>14</v>
       </c>
@@ -55210,144 +55232,144 @@
     <mergeCell ref="A61:N61"/>
   </mergeCells>
   <conditionalFormatting sqref="E43:E50">
-    <cfRule type="expression" dxfId="401" priority="32">
+    <cfRule type="expression" dxfId="425" priority="32">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="400" priority="31">
+    <cfRule type="expression" dxfId="424" priority="31">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="399" priority="30">
+    <cfRule type="expression" dxfId="423" priority="30">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="398" priority="29">
+    <cfRule type="expression" dxfId="422" priority="29">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E56">
-    <cfRule type="expression" dxfId="397" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="421" priority="1" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="396" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="420" priority="2" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="395" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="419" priority="3" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="394" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="418" priority="4" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59:E60">
-    <cfRule type="expression" dxfId="393" priority="24">
+    <cfRule type="expression" dxfId="417" priority="24">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="392" priority="21">
+    <cfRule type="expression" dxfId="416" priority="21">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="391" priority="22">
+    <cfRule type="expression" dxfId="415" priority="22">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="390" priority="23">
+    <cfRule type="expression" dxfId="414" priority="23">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="389" priority="13">
+    <cfRule type="expression" dxfId="413" priority="13">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="388" priority="14">
+    <cfRule type="expression" dxfId="412" priority="14">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="387" priority="15">
+    <cfRule type="expression" dxfId="411" priority="15">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="386" priority="16">
+    <cfRule type="expression" dxfId="410" priority="16">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16:G21 E23:G27">
-    <cfRule type="expression" dxfId="383" priority="37">
+    <cfRule type="expression" dxfId="407" priority="37">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="382" priority="38">
+    <cfRule type="expression" dxfId="406" priority="38">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:H21 H23:H27">
-    <cfRule type="expression" dxfId="379" priority="39">
+    <cfRule type="expression" dxfId="403" priority="39">
       <formula>#REF!&gt;$G16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="378" priority="40">
+    <cfRule type="expression" dxfId="402" priority="40">
       <formula>#REF!&lt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43:H50">
-    <cfRule type="expression" dxfId="377" priority="33">
+    <cfRule type="expression" dxfId="401" priority="33">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="376" priority="35">
+    <cfRule type="expression" dxfId="400" priority="35">
       <formula>#REF!&gt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="375" priority="36">
+    <cfRule type="expression" dxfId="399" priority="36">
       <formula>#REF!&lt;$G43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="374" priority="34">
+    <cfRule type="expression" dxfId="398" priority="34">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:H54 H56">
-    <cfRule type="expression" dxfId="373" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="397" priority="7" stopIfTrue="1">
       <formula>#REF!&gt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="372" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="396" priority="8" stopIfTrue="1">
       <formula>#REF!&lt;$G53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="371" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="395" priority="6" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="370" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="394" priority="5" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55">
-    <cfRule type="expression" dxfId="369" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="393" priority="10" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="368" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="392" priority="9" stopIfTrue="1">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="367" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="391" priority="12" stopIfTrue="1">
       <formula>#REF!&gt;$G55</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="366" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="390" priority="11" stopIfTrue="1">
       <formula>#REF!&lt;$G55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H60">
-    <cfRule type="expression" dxfId="365" priority="25">
+    <cfRule type="expression" dxfId="389" priority="25">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="364" priority="26">
+    <cfRule type="expression" dxfId="388" priority="26">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="363" priority="27">
+    <cfRule type="expression" dxfId="387" priority="27">
       <formula>#REF!&gt;$G59</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="362" priority="28">
+    <cfRule type="expression" dxfId="386" priority="28">
       <formula>#REF!&lt;$G59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H63">
-    <cfRule type="expression" dxfId="361" priority="20">
+    <cfRule type="expression" dxfId="385" priority="20">
       <formula>#REF!&lt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="360" priority="18">
+    <cfRule type="expression" dxfId="384" priority="18">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="359" priority="19">
+    <cfRule type="expression" dxfId="383" priority="19">
       <formula>#REF!&gt;$G63</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="358" priority="17">
+    <cfRule type="expression" dxfId="382" priority="17">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>